<commit_message>
Fixed URL of Mozambique server
</commit_message>
<xml_diff>
--- a/LookupFiles/countrySpecificVariables.xlsx
+++ b/LookupFiles/countrySpecificVariables.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ssbno-my.sharepoint.com/personal/aae_ssb_no/Documents/Documents/GitHub/ENERGY/LookupFiles/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\ENERGY\LookupFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{F5C91B66-9AD4-4B4C-9AB8-799F351C93FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D702D850-5693-46C8-A14C-4E83B33B2CCC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426DEEFD-96AC-4D93-A46D-84D0B90DF00B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2055" yWindow="1770" windowWidth="23940" windowHeight="12525" xr2:uid="{F1847B43-A334-4A7D-A69B-4F79F35D8AF5}"/>
   </bookViews>
@@ -129,9 +129,6 @@
     <t>Viken energi</t>
   </si>
   <si>
-    <t>http://41.94.86.4/energia/api</t>
-  </si>
-  <si>
     <t>SuperSaver Al Wood</t>
   </si>
   <si>
@@ -145,6 +142,9 @@
   </si>
   <si>
     <t>devicePrice</t>
+  </si>
+  <si>
+    <t>http://41.94.86.3:8080/Energy/api</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,13 +587,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>24</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -616,7 +616,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>3300</v>
@@ -657,13 +657,13 @@
         <v>41000</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3">
         <v>75000</v>
       </c>
       <c r="H3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I3">
         <v>40000</v>

</xml_diff>

<commit_message>
Update de Energy App
We upgraded the CAPI on both questonarios.
</commit_message>
<xml_diff>
--- a/LookupFiles/countrySpecificVariables.xlsx
+++ b/LookupFiles/countrySpecificVariables.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\ENERGY\LookupFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSB\ENERGY\LookupFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426DEEFD-96AC-4D93-A46D-84D0B90DF00B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1770" windowWidth="23940" windowHeight="12525" xr2:uid="{F1847B43-A334-4A7D-A69B-4F79F35D8AF5}"/>
+    <workbookView xWindow="2060" yWindow="1770" windowWidth="23940" windowHeight="12530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -144,14 +143,14 @@
     <t>devicePrice</t>
   </si>
   <si>
-    <t>http://41.94.86.3:8080/Energy/api</t>
+    <t>http://41.94.86.4:81/energia/api</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,28 +557,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A4B543-34CC-4E2A-B04F-4BB55DF5B4D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="28.5" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +610,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -640,7 +639,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -672,7 +671,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -701,37 +700,37 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="31.5">
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="17.5">
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6">
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:6">
       <c r="F18" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" tooltip="http://196.192.78.160:81/energy/api/" xr:uid="{F270E12A-E643-48D8-838A-C87F6259D9E2}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{BEE03A63-1EB2-43D0-830E-51D22A68493A}"/>
+    <hyperlink ref="B3" r:id="rId1" tooltip="http://196.192.78.160:81/energy/api/"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>

</xml_diff>

<commit_message>
Updates for Moz training
</commit_message>
<xml_diff>
--- a/LookupFiles/countrySpecificVariables.xlsx
+++ b/LookupFiles/countrySpecificVariables.xlsx
@@ -55,52 +55,6 @@
     <t>elCompany</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">COUNTRY </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">SPECIFIC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Aspirational wood ICS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">COUNTRY </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t xml:space="preserve">SPECIFIC </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Consolas"/>
-        <family val="3"/>
-      </rPr>
-      <t>Aspirational charcoal ICS</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">EDM </t>
   </si>
   <si>
@@ -144,13 +98,19 @@
   </si>
   <si>
     <t>http://41.94.86.4:81/energia/api</t>
+  </si>
+  <si>
+    <t>Chitetezo wood burner</t>
+  </si>
+  <si>
+    <t>Envirofit CH-2200 charcool cookstove</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,12 +121,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -215,29 +169,29 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -561,7 +515,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
@@ -586,13 +540,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>23</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -615,36 +569,39 @@
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>30000</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2">
+        <v>300</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2">
-        <v>3300</v>
-      </c>
-      <c r="E2">
-        <v>1100</v>
-      </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2">
+        <v>3000</v>
+      </c>
+      <c r="J2" t="s">
         <v>8</v>
-      </c>
-      <c r="G2">
-        <v>1100</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>1100</v>
-      </c>
-      <c r="J2" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="C3">
         <v>272000</v>
@@ -656,27 +613,27 @@
         <v>41000</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G3">
         <v>75000</v>
       </c>
       <c r="H3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I3">
         <v>40000</v>
       </c>
       <c r="J3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>50000</v>
@@ -685,19 +642,19 @@
         <v>5000</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4">
         <v>10000</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="I4">
         <v>3000</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="31.8">

</xml_diff>

<commit_message>
Got rid of the "energia" in the url of the server
</commit_message>
<xml_diff>
--- a/LookupFiles/countrySpecificVariables.xlsx
+++ b/LookupFiles/countrySpecificVariables.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SSB\ENERGY\LookupFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\github\ENERGY\LookupFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A284EA0A-7018-43B8-997B-75BAC0CD193F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2064" yWindow="1776" windowWidth="23940" windowHeight="12528"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,11 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -97,20 +93,20 @@
     <t>devicePrice</t>
   </si>
   <si>
-    <t>http://41.94.86.4:81/energia/api</t>
-  </si>
-  <si>
     <t>Chitetezo wood burner</t>
   </si>
   <si>
     <t>Envirofit CH-2200 charcool cookstove</t>
+  </si>
+  <si>
+    <t>http://41.94.86.4:81/Energy/api</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -511,28 +507,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="40" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.5" customHeight="1">
+    <row r="1" spans="1:10" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -564,12 +560,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -581,13 +577,13 @@
         <v>30000</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2">
         <v>300</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I2">
         <v>3000</v>
@@ -596,7 +592,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -628,7 +624,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -657,37 +653,37 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="31.8">
+    <row r="10" spans="1:10" ht="31.5" x14ac:dyDescent="0.25">
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:10" ht="17.399999999999999">
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.25">
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F12" s="7"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F15" s="4"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F16" s="4"/>
     </row>
-    <row r="17" spans="6:6">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="6:6">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
       <c r="F18" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" tooltip="http://196.192.78.160:81/energy/api/"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B3" r:id="rId1" tooltip="http://196.192.78.160:81/energy/api/" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>

</xml_diff>